<commit_message>
add 197555 and 50159 appendices. minor changes to functions
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A41F917-60A4-4A20-B78F-BF90FB56784F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04123B79-41A8-4BBA-8CFE-50D86D388165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
   <si>
     <t>hab_value</t>
   </si>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -632,8 +632,14 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
       <c r="J2" t="s">
         <v>52</v>
+      </c>
+      <c r="M2">
+        <v>6000</v>
       </c>
       <c r="N2" t="s">
         <v>49</v>
@@ -655,6 +661,9 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="H3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -732,7 +741,7 @@
         <v>35</v>
       </c>
       <c r="M8">
-        <v>0.125</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -841,8 +850,14 @@
       <c r="D15">
         <v>400</v>
       </c>
+      <c r="H15" t="s">
+        <v>31</v>
+      </c>
       <c r="J15" t="s">
         <v>31</v>
+      </c>
+      <c r="M15">
+        <v>350</v>
       </c>
       <c r="O15" t="s">
         <v>9</v>
@@ -861,6 +876,9 @@
       <c r="D16">
         <v>150</v>
       </c>
+      <c r="H16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -884,6 +902,9 @@
       <c r="J17" t="s">
         <v>52</v>
       </c>
+      <c r="M17">
+        <v>1800</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -943,8 +964,14 @@
       <c r="E21" t="s">
         <v>9</v>
       </c>
+      <c r="H21" t="s">
+        <v>31</v>
+      </c>
       <c r="J21" t="s">
         <v>52</v>
+      </c>
+      <c r="M21">
+        <v>4500</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -962,6 +989,9 @@
       </c>
       <c r="E22" t="s">
         <v>9</v>
+      </c>
+      <c r="H22" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add a summary table for hab
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04123B79-41A8-4BBA-8CFE-50D86D388165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC73ED14-54FC-435F-A39F-024223CFEAFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
   <si>
     <t>hab_value</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>moderate</t>
+  </si>
+  <si>
+    <t>EB, WCT</t>
   </si>
 </sst>
 </file>
@@ -552,8 +555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -905,6 +908,9 @@
       <c r="M17">
         <v>1800</v>
       </c>
+      <c r="N17" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
@@ -973,6 +979,9 @@
       <c r="M21">
         <v>4500</v>
       </c>
+      <c r="N21" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -1007,11 +1016,17 @@
       <c r="D23">
         <v>730</v>
       </c>
+      <c r="H23" t="s">
+        <v>31</v>
+      </c>
       <c r="J23" t="s">
         <v>52</v>
       </c>
       <c r="K23" t="s">
         <v>36</v>
+      </c>
+      <c r="M23">
+        <v>540</v>
       </c>
       <c r="O23" t="s">
         <v>9</v>
@@ -1029,6 +1044,9 @@
       </c>
       <c r="D24">
         <v>630</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move to pagedown.  add css styles for pagedown.
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38F883D-CFF3-448B-B3E5-1C1793620168}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EBACD1-FE80-4E45-A677-8CE38AE0D3B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
   <si>
     <t>hab_value</t>
   </si>
@@ -185,9 +185,6 @@
     <t>BT</t>
   </si>
   <si>
-    <t>BT, WCT</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
@@ -195,6 +192,12 @@
   </si>
   <si>
     <t>EB, WCT</t>
+  </si>
+  <si>
+    <t>RB, WCT</t>
+  </si>
+  <si>
+    <t>RB, WCT, BT</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A11:XFD11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -639,7 +642,7 @@
         <v>31</v>
       </c>
       <c r="J2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M2">
         <v>6000</v>
@@ -701,16 +704,19 @@
         <v>39</v>
       </c>
       <c r="D6">
-        <v>980</v>
+        <v>1600</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -737,6 +743,9 @@
       <c r="D8">
         <v>125</v>
       </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
       <c r="J8" t="s">
         <v>31</v>
       </c>
@@ -745,6 +754,9 @@
       </c>
       <c r="M8">
         <v>125</v>
+      </c>
+      <c r="N8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -760,6 +772,9 @@
       <c r="D9">
         <v>400</v>
       </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -792,7 +807,7 @@
         <v>725</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J11" t="s">
         <v>32</v>
@@ -815,10 +830,10 @@
         <v>650</v>
       </c>
       <c r="H12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" t="s">
         <v>51</v>
-      </c>
-      <c r="J12" t="s">
-        <v>52</v>
       </c>
       <c r="M12">
         <v>1800</v>
@@ -841,7 +856,7 @@
         <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M13">
         <v>170</v>
@@ -927,13 +942,13 @@
         <v>31</v>
       </c>
       <c r="J17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M17">
         <v>1800</v>
       </c>
       <c r="N17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -953,7 +968,7 @@
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -998,13 +1013,13 @@
         <v>31</v>
       </c>
       <c r="J21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M21">
         <v>4500</v>
       </c>
       <c r="N21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1044,7 +1059,7 @@
         <v>31</v>
       </c>
       <c r="J23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K23" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
move the pase 1 appendix to the end to deal with pagedown render issue and add printable.html download link as test
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EBACD1-FE80-4E45-A677-8CE38AE0D3B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB36189-0A83-4ADF-9B6F-B4C472867387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -715,6 +715,9 @@
       <c r="J6" t="s">
         <v>51</v>
       </c>
+      <c r="M6">
+        <v>23000</v>
+      </c>
       <c r="N6" t="s">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
new geopackage, changed outgoing-mapping function to overwrite, tweaked hab tables to include reference, added nupku sites to input spreadsheet
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB36189-0A83-4ADF-9B6F-B4C472867387}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB715D-9543-471B-97FE-008FA4935761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
   <si>
     <t>hab_value</t>
   </si>
@@ -107,12 +107,6 @@
     <t>50155_ds</t>
   </si>
   <si>
-    <t>50155_us_ef</t>
-  </si>
-  <si>
-    <t>50155_ds_ef</t>
-  </si>
-  <si>
     <t>Unnamed Tributary to Morrissey Creek</t>
   </si>
   <si>
@@ -164,12 +158,6 @@
     <t>197559_us_ef</t>
   </si>
   <si>
-    <t>197555_ds_ef</t>
-  </si>
-  <si>
-    <t>197555_us_ef</t>
-  </si>
-  <si>
     <t>recommendation</t>
   </si>
   <si>
@@ -198,6 +186,54 @@
   </si>
   <si>
     <t>RB, WCT, BT</t>
+  </si>
+  <si>
+    <t>Hartley Creek</t>
+  </si>
+  <si>
+    <t>197542_us</t>
+  </si>
+  <si>
+    <t>197542_ds</t>
+  </si>
+  <si>
+    <t>197582_ds</t>
+  </si>
+  <si>
+    <t>50181_us</t>
+  </si>
+  <si>
+    <t>50181_ds</t>
+  </si>
+  <si>
+    <t>Stove Creek</t>
+  </si>
+  <si>
+    <t>50152_us</t>
+  </si>
+  <si>
+    <t>Weigart Creek</t>
+  </si>
+  <si>
+    <t>197534_us</t>
+  </si>
+  <si>
+    <t>197534_ds</t>
+  </si>
+  <si>
+    <t>Unnamed Tributary to Michel Creek</t>
+  </si>
+  <si>
+    <t>50261_us</t>
+  </si>
+  <si>
+    <t>50261_ds</t>
+  </si>
+  <si>
+    <t>no fix</t>
+  </si>
+  <si>
+    <t>50152_ds</t>
   </si>
 </sst>
 </file>
@@ -213,18 +249,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -239,9 +269,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -601,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
         <v>1</v>
@@ -610,16 +639,16 @@
         <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -630,7 +659,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>675</v>
@@ -639,16 +668,16 @@
         <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M2">
         <v>6000</v>
       </c>
       <c r="N2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -659,7 +688,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>700</v>
@@ -668,427 +697,600 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>1600</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4">
+        <v>23000</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6">
-        <v>1600</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
       </c>
       <c r="M6">
-        <v>23000</v>
+        <v>125</v>
       </c>
       <c r="N6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>400</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="D8">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" t="s">
-        <v>35</v>
-      </c>
-      <c r="M8">
-        <v>125</v>
-      </c>
-      <c r="N8" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D9">
-        <v>400</v>
+        <v>725</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9">
+        <v>2400</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>30</v>
+        <v>650</v>
       </c>
       <c r="H10" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10">
+        <v>1800</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>725</v>
+        <v>170</v>
       </c>
       <c r="H11" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="J11" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="M11">
-        <v>2400</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12">
-        <v>650</v>
+        <v>75</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12">
-        <v>1800</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>170</v>
+        <v>400</v>
       </c>
       <c r="H13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J13" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M13">
-        <v>170</v>
+        <v>350</v>
+      </c>
+      <c r="O13" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D14">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15">
-        <v>400</v>
+        <v>700</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
       </c>
       <c r="H15" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="M15">
-        <v>350</v>
-      </c>
-      <c r="O15" t="s">
-        <v>9</v>
+        <v>1800</v>
+      </c>
+      <c r="N15" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D16">
-        <v>150</v>
+        <v>100</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>700</v>
+        <v>740</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="H17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M17">
-        <v>1800</v>
+        <v>4500</v>
       </c>
       <c r="N17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D18">
-        <v>100</v>
+        <v>255</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>730</v>
+      </c>
+      <c r="H19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J19" t="s">
+        <v>47</v>
+      </c>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19">
+        <v>540</v>
+      </c>
+      <c r="O19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>630</v>
+      </c>
+      <c r="H20" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D21">
-        <v>740</v>
-      </c>
-      <c r="E21" t="s">
-        <v>9</v>
+        <v>725</v>
       </c>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="M21">
-        <v>4500</v>
-      </c>
-      <c r="N21" t="s">
-        <v>52</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="D22">
-        <v>255</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
+        <v>900</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D23">
-        <v>730</v>
+        <v>540</v>
       </c>
       <c r="H23" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23" t="s">
-        <v>51</v>
-      </c>
-      <c r="K23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M23">
-        <v>540</v>
-      </c>
-      <c r="O23" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D24">
-        <v>630</v>
+        <v>515</v>
       </c>
       <c r="H24" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25">
+        <v>200</v>
+      </c>
+      <c r="H25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26">
+        <v>675</v>
+      </c>
+      <c r="H26" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>140</v>
+      </c>
+      <c r="H27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>1100</v>
+      </c>
+      <c r="H28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="M28">
+        <v>11600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29">
+        <v>675</v>
+      </c>
+      <c r="H29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30">
+        <v>220</v>
+      </c>
+      <c r="H30" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" t="s">
+        <v>65</v>
+      </c>
+      <c r="M30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>45</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31">
+        <v>210</v>
+      </c>
+      <c r="H31" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish hartley, add weigert and michel
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93BB715D-9543-471B-97FE-008FA4935761}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DC5905-C066-4028-948F-2C103B314F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,13 +588,13 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" customWidth="1"/>
     <col min="4" max="4" width="14.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
@@ -1110,7 +1110,7 @@
         <v>53</v>
       </c>
       <c r="D22">
-        <v>900</v>
+        <v>400</v>
       </c>
       <c r="H22" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
update text, shift position of phase 1 appendix
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DC5905-C066-4028-948F-2C103B314F80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A9D0C4-82BC-4575-8BDF-5BD1B5AEB845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="82">
   <si>
     <t>hab_value</t>
   </si>
@@ -134,9 +134,6 @@
     <t>future_sampling_recommended</t>
   </si>
   <si>
-    <t>Deactivate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fry observed upstream and downstream </t>
   </si>
   <si>
@@ -164,9 +161,6 @@
     <t>upstream_habitat_length_m</t>
   </si>
   <si>
-    <t>habitat_value_rationale</t>
-  </si>
-  <si>
     <t>species_codes</t>
   </si>
   <si>
@@ -234,6 +228,57 @@
   </si>
   <si>
     <t>50152_ds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recommend exploring deactivation as a potential remediatory action. Culvert is located 125m below crossing 197559.  </t>
+  </si>
+  <si>
+    <t>Crossing dry at time of survey.  Incorrectly mapped as Grave Creek.  Steep gradients in Harriet Lake Creek approximatlely 1km upstream.</t>
+  </si>
+  <si>
+    <t>Deep pools, large woody debris and boulders present.  Stream is Grave Creek mainstem that has redirected from historic channel. Higher value habitat in adjacent valley channel. Crossing is 170m downstream of 62426. Westslope cutthrout density study underway within watershed by Lotic Environmental Ltd.</t>
+  </si>
+  <si>
+    <t>Deep pools, boulders and undercut banks within wetted channel upstream.  Adult westslope cutthout trout in outlet pool below hwy. Section of stream (670m) immediately upstream of Highway 43 subsurface during survey.  Electrofished upstream only with no fish captured.</t>
+  </si>
+  <si>
+    <t>Good flows, pools to 0.6m deep and pockets of gravel suitable for spawning. Infrequent large woody debris jams to 0.5m high.  Sites electrofished upstream and downstream with one bull trout captured downstream within 315m site.</t>
+  </si>
+  <si>
+    <t>Deep pools, large woody debris and boulders present.  Habitat quality decreases with distance upstream.  Upstream tributary too steep at 250m upstream.  Channel is Grave Creek mainstem that has redirected from historic channel. Culvert is 170m usptream of 62425.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good flows, pools to 0.6m deep and pockets of gravel suitable for salmonid spawning throughout.  Infrequent large woody debris jams to 0.5m high.  Electrofishing indicated generally higher densities of fry, parr and juvenile westslope cutthrout trout downstream when compared to upstream. </t>
+  </si>
+  <si>
+    <t>(WCT)</t>
+  </si>
+  <si>
+    <t>Frequent pools formed by small and large woody debris ranging from 0.3 - 0.7m in depth. Pockets of gravels suitable for resident and fluvial salmonids. Downstream crossing on Hwy 3 is passable but requires dredging to keep clear.  Historic fish density information available on Ecocat for 3 upstream sites.</t>
+  </si>
+  <si>
+    <t>WCT, BT, EB</t>
+  </si>
+  <si>
+    <t>WCT</t>
+  </si>
+  <si>
+    <t>Undercut banks, small woody debris, large woody debris, boulders, deep pools, and overhanging vegetation present.  Abundant gravels present. Habitat  increasingly complex upstream. Watershed is a habitat protection area with motor vehicle restrictions. Elk Valley Park recreation site is located downstream of the crossing.</t>
+  </si>
+  <si>
+    <t>A 4.4m high chute was located 200m downstream of crossing (UTM: 11U 668858 5481210) and is considered a permanent impassable barrier to upstream migration.</t>
+  </si>
+  <si>
+    <t>Newly installed culvert with large outlet drop.  Cover as undercut banks, small woody debris, large woody debris and overhanging vegetation.  Numerous fry observed throughout the area surveyed and abundant gravels suitable for salmonid spawning. Highest value habitat of 4 Lizard Creek tributary streams surveyed.</t>
+  </si>
+  <si>
+    <t>Frequent areas of gravels suitable for resident westslope cutthrout trout spawning and pools to 40cm deep associated with small and large woody debris. Fish sampling indicates westslope cutthrout trout fry densities lower upstream than downstream.</t>
+  </si>
+  <si>
+    <t>Abundant gravels suitable for resident and fluvial westslope cutthrout trout spawning.  Frequent pools to 40cm deep associated with woody debris.  Within old growth cedar forest and not mapped in the freshwater atlas stream layer.  Flows potentially diverted  as part of a micro-hydro facilty for Island Lake Lodge.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boulders, small woody debris, large woody debris, undercut banks, overhanging vegetation and gravels suitable for spawning.  Electrofished upstream and downstream of the crossing with westslope cutthrout trout fry, juvenile and adult fish observed downstream only.  Densities of parr lower in the steeper habitat located upstream. </t>
   </si>
 </sst>
 </file>
@@ -585,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -600,11 +645,10 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="9" max="9" width="19.875" customWidth="1"/>
-    <col min="14" max="14" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -630,13 +674,13 @@
         <v>0</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="L1" t="s">
         <v>41</v>
@@ -645,13 +689,10 @@
         <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -659,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>675</v>
@@ -670,17 +711,20 @@
       <c r="H2" t="s">
         <v>29</v>
       </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
       <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2">
+        <v>69</v>
+      </c>
+      <c r="L2">
         <v>6000</v>
       </c>
-      <c r="N2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -688,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>700</v>
@@ -700,7 +744,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -708,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>1600</v>
@@ -719,17 +763,20 @@
       <c r="H4" t="s">
         <v>29</v>
       </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
       <c r="J4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4">
+        <v>23000</v>
+      </c>
+      <c r="M4" t="s">
         <v>47</v>
       </c>
-      <c r="M4">
-        <v>23000</v>
-      </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -737,10 +784,10 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7</v>
       </c>
@@ -748,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>125</v>
@@ -756,20 +803,20 @@
       <c r="H6" t="s">
         <v>29</v>
       </c>
+      <c r="I6" t="s">
+        <v>29</v>
+      </c>
       <c r="J6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6">
+        <v>65</v>
+      </c>
+      <c r="L6">
         <v>125</v>
       </c>
-      <c r="N6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8</v>
       </c>
@@ -777,16 +824,16 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -803,7 +850,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10</v>
       </c>
@@ -817,16 +864,22 @@
         <v>725</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="L9">
+        <v>2300</v>
+      </c>
+      <c r="M9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>11</v>
       </c>
@@ -840,16 +893,22 @@
         <v>650</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="I10" t="s">
+        <v>45</v>
       </c>
       <c r="J10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M10">
+        <v>70</v>
+      </c>
+      <c r="L10">
         <v>1800</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -865,14 +924,20 @@
       <c r="H11" t="s">
         <v>29</v>
       </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
       <c r="J11" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11">
+        <v>67</v>
+      </c>
+      <c r="L11">
         <v>170</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>13</v>
       </c>
@@ -889,7 +954,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -905,17 +970,20 @@
       <c r="H13" t="s">
         <v>29</v>
       </c>
+      <c r="I13" t="s">
+        <v>45</v>
+      </c>
       <c r="J13" t="s">
-        <v>47</v>
-      </c>
-      <c r="M13">
+        <v>80</v>
+      </c>
+      <c r="L13">
         <v>350</v>
       </c>
-      <c r="O13" t="s">
+      <c r="N13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>15</v>
       </c>
@@ -932,7 +1000,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>16</v>
       </c>
@@ -951,17 +1019,20 @@
       <c r="H15" t="s">
         <v>29</v>
       </c>
+      <c r="I15" t="s">
+        <v>45</v>
+      </c>
       <c r="J15" t="s">
-        <v>47</v>
-      </c>
-      <c r="M15">
+        <v>79</v>
+      </c>
+      <c r="L15">
         <v>1800</v>
       </c>
-      <c r="N15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>17</v>
       </c>
@@ -978,10 +1049,10 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>20</v>
       </c>
@@ -1000,17 +1071,20 @@
       <c r="H17" t="s">
         <v>29</v>
       </c>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
       <c r="J17" t="s">
-        <v>47</v>
-      </c>
-      <c r="M17">
+        <v>71</v>
+      </c>
+      <c r="L17">
         <v>4500</v>
       </c>
-      <c r="N17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>21</v>
       </c>
@@ -1030,7 +1104,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>22</v>
       </c>
@@ -1046,20 +1120,23 @@
       <c r="H19" t="s">
         <v>29</v>
       </c>
+      <c r="I19" t="s">
+        <v>45</v>
+      </c>
       <c r="J19" t="s">
-        <v>47</v>
-      </c>
-      <c r="K19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19">
+        <v>33</v>
+      </c>
+      <c r="L19">
         <v>540</v>
       </c>
-      <c r="O19" t="s">
+      <c r="M19" t="s">
+        <v>72</v>
+      </c>
+      <c r="N19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>23</v>
       </c>
@@ -1076,64 +1153,73 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D21">
         <v>725</v>
       </c>
+      <c r="G21" t="s">
+        <v>9</v>
+      </c>
       <c r="H21" t="s">
         <v>29</v>
       </c>
+      <c r="I21" t="s">
+        <v>29</v>
+      </c>
       <c r="J21" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21">
+        <v>73</v>
+      </c>
+      <c r="L21">
         <v>7200</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>36</v>
       </c>
       <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
         <v>51</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
       </c>
       <c r="D22">
         <v>400</v>
       </c>
       <c r="H22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23">
         <v>540</v>
       </c>
       <c r="H23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>38</v>
       </c>
@@ -1141,22 +1227,28 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D24">
         <v>515</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="I24" t="s">
+        <v>29</v>
       </c>
       <c r="J24" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24">
+        <v>81</v>
+      </c>
+      <c r="L24">
         <v>515</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>39</v>
       </c>
@@ -1164,24 +1256,24 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D25">
         <v>200</v>
       </c>
       <c r="H25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D26">
         <v>675</v>
@@ -1189,22 +1281,28 @@
       <c r="H26" t="s">
         <v>29</v>
       </c>
+      <c r="I26" t="s">
+        <v>29</v>
+      </c>
       <c r="J26" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26">
+        <v>78</v>
+      </c>
+      <c r="L26">
         <v>2700</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D27">
         <v>140</v>
@@ -1213,15 +1311,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D28">
         <v>1100</v>
@@ -1229,68 +1327,74 @@
       <c r="H28" t="s">
         <v>29</v>
       </c>
+      <c r="I28" t="s">
+        <v>29</v>
+      </c>
       <c r="J28" t="s">
-        <v>29</v>
-      </c>
-      <c r="M28">
+        <v>76</v>
+      </c>
+      <c r="L28">
         <v>11600</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>43</v>
       </c>
       <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
         <v>59</v>
-      </c>
-      <c r="C29" t="s">
-        <v>61</v>
       </c>
       <c r="D29">
         <v>675</v>
       </c>
       <c r="H29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D30">
         <v>220</v>
       </c>
       <c r="H30" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="I30" t="s">
+        <v>63</v>
       </c>
       <c r="J30" t="s">
-        <v>65</v>
-      </c>
-      <c r="M30">
+        <v>77</v>
+      </c>
+      <c r="L30">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>45</v>
       </c>
       <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" t="s">
-        <v>64</v>
       </c>
       <c r="D31">
         <v>210</v>
       </c>
       <c r="H31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sculpt tables. first big commit since crash
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2020-025_cwf_elk\scripts\fish_passage_elk_2020_reporting_cwf\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A9D0C4-82BC-4575-8BDF-5BD1B5AEB845}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B04D2A-7CF2-4171-A784-A40BF06B1572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>future_sampling_recommended</t>
   </si>
   <si>
-    <t xml:space="preserve">Fry observed upstream and downstream </t>
-  </si>
-  <si>
     <t>197555_us</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t xml:space="preserve">Boulders, small woody debris, large woody debris, undercut banks, overhanging vegetation and gravels suitable for spawning.  Electrofished upstream and downstream of the crossing with westslope cutthrout trout fry, juvenile and adult fish observed downstream only.  Densities of parr lower in the steeper habitat located upstream. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undercut banks throughout with small woody debris, large woody debris, deep pools, and overhanging vegetation also present.  Abundant gravels suitable for resident westslope cutthrout trout spawning. Fry observed upstream and downstream. </t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
   <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -680,13 +680,13 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
         <v>40</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
       </c>
       <c r="N1" t="s">
         <v>32</v>
@@ -700,7 +700,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>675</v>
@@ -712,16 +712,16 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L2">
         <v>6000</v>
       </c>
       <c r="M2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3">
         <v>700</v>
@@ -752,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>1600</v>
@@ -764,16 +764,16 @@
         <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L4">
         <v>23000</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>125</v>
@@ -807,13 +807,13 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L6">
         <v>125</v>
       </c>
       <c r="M6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -824,13 +824,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>400</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -864,19 +864,19 @@
         <v>725</v>
       </c>
       <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" t="s">
-        <v>45</v>
-      </c>
       <c r="J9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L9">
         <v>2300</v>
       </c>
       <c r="M9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -893,19 +893,19 @@
         <v>650</v>
       </c>
       <c r="H10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" t="s">
         <v>44</v>
       </c>
-      <c r="I10" t="s">
-        <v>45</v>
-      </c>
       <c r="J10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L10">
         <v>1800</v>
       </c>
       <c r="M10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -925,16 +925,16 @@
         <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L11">
         <v>170</v>
       </c>
       <c r="M11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -971,10 +971,10 @@
         <v>29</v>
       </c>
       <c r="I13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L13">
         <v>350</v>
@@ -1020,16 +1020,16 @@
         <v>29</v>
       </c>
       <c r="I15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L15">
         <v>1800</v>
       </c>
       <c r="M15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1049,7 +1049,7 @@
         <v>9</v>
       </c>
       <c r="H16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -1072,16 +1072,16 @@
         <v>29</v>
       </c>
       <c r="I17" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="J17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L17">
         <v>4500</v>
       </c>
       <c r="M17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -1121,16 +1121,16 @@
         <v>29</v>
       </c>
       <c r="I19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J19" t="s">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="L19">
         <v>540</v>
       </c>
       <c r="M19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N19" t="s">
         <v>9</v>
@@ -1158,10 +1158,10 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
       </c>
       <c r="D21">
         <v>725</v>
@@ -1176,13 +1176,13 @@
         <v>29</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L21">
         <v>7200</v>
       </c>
       <c r="M21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1190,16 +1190,16 @@
         <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D22">
         <v>400</v>
       </c>
       <c r="H22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1207,16 +1207,16 @@
         <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>540</v>
       </c>
       <c r="H23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1227,25 +1227,25 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24">
         <v>515</v>
       </c>
       <c r="H24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I24" t="s">
         <v>29</v>
       </c>
       <c r="J24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L24">
         <v>515</v>
       </c>
       <c r="M24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1256,13 +1256,13 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25">
         <v>200</v>
       </c>
       <c r="H25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1270,10 +1270,10 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>56</v>
       </c>
       <c r="D26">
         <v>675</v>
@@ -1285,13 +1285,13 @@
         <v>29</v>
       </c>
       <c r="J26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L26">
         <v>2700</v>
       </c>
       <c r="M26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1299,10 +1299,10 @@
         <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27">
         <v>140</v>
@@ -1316,10 +1316,10 @@
         <v>42</v>
       </c>
       <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
         <v>57</v>
-      </c>
-      <c r="C28" t="s">
-        <v>58</v>
       </c>
       <c r="D28">
         <v>1100</v>
@@ -1331,7 +1331,7 @@
         <v>29</v>
       </c>
       <c r="J28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L28">
         <v>11600</v>
@@ -1342,16 +1342,16 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <v>675</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1359,22 +1359,22 @@
         <v>44</v>
       </c>
       <c r="B30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" t="s">
-        <v>61</v>
       </c>
       <c r="D30">
         <v>220</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L30">
         <v>0</v>
@@ -1385,16 +1385,16 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D31">
         <v>210</v>
       </c>
       <c r="H31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SWITCH TO PSCIS IDS!!
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9788C246-2EEA-4AA9-A08F-5D4D7445FBB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C7068-94F9-4592-89DF-3DDB2558BF4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
   <si>
     <t>hab_value</t>
   </si>
@@ -74,45 +74,15 @@
     <t>Unnamed Tributary to Buck Creek</t>
   </si>
   <si>
-    <t>1800092_ds</t>
-  </si>
-  <si>
-    <t>1800092_us</t>
-  </si>
-  <si>
     <t>Byman Creek</t>
   </si>
   <si>
-    <t>1800062_us</t>
-  </si>
-  <si>
-    <t>1800062_ds2</t>
-  </si>
-  <si>
-    <t>1800062_ds1</t>
-  </si>
-  <si>
     <t>Richfield Creek</t>
   </si>
   <si>
-    <t>1800060_us</t>
-  </si>
-  <si>
-    <t>1800060_ds</t>
-  </si>
-  <si>
     <t>Barren Creek</t>
   </si>
   <si>
-    <t>1801069_us</t>
-  </si>
-  <si>
-    <t>1801069_ds</t>
-  </si>
-  <si>
-    <t>1800076_ds</t>
-  </si>
-  <si>
     <t>Tyhee Creek</t>
   </si>
   <si>
@@ -146,9 +116,6 @@
     <t>Coffin Creek</t>
   </si>
   <si>
-    <t>1805608_ds</t>
-  </si>
-  <si>
     <t>3042_us</t>
   </si>
   <si>
@@ -170,12 +137,6 @@
     <t>3054_us</t>
   </si>
   <si>
-    <t>1800213_us</t>
-  </si>
-  <si>
-    <t>1800213_ds</t>
-  </si>
-  <si>
     <t>58159_ds</t>
   </si>
   <si>
@@ -240,6 +201,48 @@
   </si>
   <si>
     <t>reference_number</t>
+  </si>
+  <si>
+    <t>197640_ds</t>
+  </si>
+  <si>
+    <t>197640_us</t>
+  </si>
+  <si>
+    <t>197658_us</t>
+  </si>
+  <si>
+    <t>197658_ds2</t>
+  </si>
+  <si>
+    <t>197658_ds1</t>
+  </si>
+  <si>
+    <t>197662_us</t>
+  </si>
+  <si>
+    <t>197662_ds</t>
+  </si>
+  <si>
+    <t>197664_us</t>
+  </si>
+  <si>
+    <t>197664_ds</t>
+  </si>
+  <si>
+    <t>197665_ds</t>
+  </si>
+  <si>
+    <t>197668_ds</t>
+  </si>
+  <si>
+    <t>197663_us</t>
+  </si>
+  <si>
+    <t>197663_ds</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -591,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -609,25 +612,25 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>
@@ -639,13 +642,13 @@
         <v>2</v>
       </c>
       <c r="K1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="M1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -740,7 +743,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>70</v>
@@ -754,7 +757,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="D9">
         <v>535</v>
@@ -765,16 +768,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="D10">
         <v>1400</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -782,10 +785,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>330</v>
@@ -796,16 +799,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>300</v>
       </c>
       <c r="F12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -813,16 +816,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="D13">
         <v>1200</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -830,16 +833,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -847,10 +850,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D15">
         <v>800</v>
@@ -861,10 +864,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D16">
         <v>240</v>
@@ -875,10 +878,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="D17">
         <v>20</v>
@@ -889,10 +892,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D18">
         <v>170</v>
@@ -903,10 +906,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="D19">
         <v>540</v>
@@ -917,10 +920,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>100</v>
@@ -931,10 +934,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>1100</v>
@@ -945,10 +948,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D22">
         <v>415</v>
@@ -959,16 +962,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D23">
         <v>520</v>
       </c>
       <c r="F23" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -976,16 +979,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D24">
         <v>450</v>
       </c>
       <c r="F24" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -993,16 +996,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D25">
         <v>300</v>
       </c>
       <c r="F25" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,16 +1013,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D26">
         <v>415</v>
       </c>
       <c r="F26" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,10 +1030,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D27">
         <v>400</v>
@@ -1041,10 +1044,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D28">
         <v>260</v>
@@ -1055,16 +1058,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C29" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D29">
         <v>285</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1072,16 +1075,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D30">
         <v>625</v>
       </c>
       <c r="E30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1089,10 +1092,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D31">
         <v>350</v>
@@ -1103,187 +1106,192 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="D32">
         <v>725</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="D33">
         <v>690</v>
       </c>
       <c r="E33" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D34">
         <v>300</v>
       </c>
       <c r="E34" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D35">
         <v>135</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D36">
         <v>440</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D37">
         <v>150</v>
       </c>
       <c r="E37" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F37" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D38">
         <v>150</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F38" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D39">
         <v>250</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D40">
         <v>300</v>
       </c>
       <c r="E40" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D41">
         <v>1200</v>
       </c>
       <c r="E41" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="G41" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H46" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorg file to run minimal with first build w bulkley data
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A8C7068-94F9-4592-89DF-3DDB2558BF4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6CAEC-444A-41CF-AA23-EE1234B39E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -596,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add hydrometric and draft priority levels.  Clean text
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A6CAEC-444A-41CF-AA23-EE1234B39E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB2910-741D-402B-A08F-2D342104E722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t>hab_value</t>
   </si>
@@ -243,6 +243,15 @@
   </si>
   <si>
     <t>`</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>low</t>
   </si>
 </sst>
 </file>
@@ -596,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -692,6 +701,12 @@
       <c r="D4">
         <v>525</v>
       </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -706,6 +721,12 @@
       <c r="D5">
         <v>650</v>
       </c>
+      <c r="I5" t="s">
+        <v>70</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -720,6 +741,9 @@
       <c r="D6">
         <v>540</v>
       </c>
+      <c r="I6" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -762,6 +786,12 @@
       <c r="D9">
         <v>535</v>
       </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -779,6 +809,12 @@
       <c r="F10" t="s">
         <v>51</v>
       </c>
+      <c r="I10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -827,6 +863,12 @@
       <c r="F13" t="s">
         <v>51</v>
       </c>
+      <c r="I13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -858,6 +900,9 @@
       <c r="D15">
         <v>800</v>
       </c>
+      <c r="I15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -873,7 +918,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -887,7 +932,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -901,7 +946,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -914,8 +959,11 @@
       <c r="D19">
         <v>540</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -928,8 +976,11 @@
       <c r="D20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -942,8 +993,11 @@
       <c r="D21">
         <v>1100</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -957,7 +1011,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -973,8 +1027,11 @@
       <c r="F23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -991,7 +1048,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1008,7 +1065,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1024,8 +1081,14 @@
       <c r="F26" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>71</v>
+      </c>
+      <c r="M26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1038,8 +1101,14 @@
       <c r="D27">
         <v>400</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1053,7 +1122,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1070,7 +1139,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1086,8 +1155,11 @@
       <c r="E30" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1101,7 +1173,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1114,8 +1186,11 @@
       <c r="D32">
         <v>725</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1134,8 +1209,11 @@
       <c r="F33" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1155,7 +1233,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1172,7 +1250,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1188,8 +1266,11 @@
       <c r="E36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1209,7 +1290,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1231,8 +1312,11 @@
       <c r="G38" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1249,7 +1333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1269,7 +1353,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1288,8 +1372,11 @@
       <c r="G41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H46" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
add upstream sites missed
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EB2910-741D-402B-A08F-2D342104E722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02946E4-3609-4F0B-A805-9EE244014FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="76">
   <si>
     <t>hab_value</t>
   </si>
@@ -242,9 +242,6 @@
     <t>197663_ds</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>moderate</t>
   </si>
   <si>
@@ -252,6 +249,18 @@
   </si>
   <si>
     <t>low</t>
+  </si>
+  <si>
+    <t>195288_us</t>
+  </si>
+  <si>
+    <t>197665_us</t>
+  </si>
+  <si>
+    <t>197667_us</t>
+  </si>
+  <si>
+    <t>197668_us</t>
   </si>
 </sst>
 </file>
@@ -603,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -702,7 +711,7 @@
         <v>525</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M4" t="s">
         <v>51</v>
@@ -722,7 +731,7 @@
         <v>650</v>
       </c>
       <c r="I5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M5" t="s">
         <v>51</v>
@@ -742,7 +751,7 @@
         <v>540</v>
       </c>
       <c r="I6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -787,7 +796,7 @@
         <v>535</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M9" t="s">
         <v>51</v>
@@ -810,7 +819,7 @@
         <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M10" t="s">
         <v>51</v>
@@ -864,7 +873,7 @@
         <v>51</v>
       </c>
       <c r="I13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M13" t="s">
         <v>51</v>
@@ -901,7 +910,7 @@
         <v>800</v>
       </c>
       <c r="I15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -960,7 +969,7 @@
         <v>540</v>
       </c>
       <c r="I19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -977,7 +986,7 @@
         <v>100</v>
       </c>
       <c r="I20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -994,7 +1003,7 @@
         <v>1100</v>
       </c>
       <c r="I21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1028,7 +1037,7 @@
         <v>51</v>
       </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -1082,7 +1091,7 @@
         <v>51</v>
       </c>
       <c r="I26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M26" t="s">
         <v>51</v>
@@ -1102,7 +1111,7 @@
         <v>400</v>
       </c>
       <c r="I27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M27" t="s">
         <v>51</v>
@@ -1156,7 +1165,7 @@
         <v>51</v>
       </c>
       <c r="I30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
@@ -1187,7 +1196,7 @@
         <v>725</v>
       </c>
       <c r="I32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -1210,7 +1219,7 @@
         <v>51</v>
       </c>
       <c r="I33" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1267,7 +1276,7 @@
         <v>51</v>
       </c>
       <c r="I36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -1313,7 +1322,7 @@
         <v>51</v>
       </c>
       <c r="I38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -1373,12 +1382,75 @@
         <v>51</v>
       </c>
       <c r="I41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43">
+        <v>100</v>
+      </c>
+      <c r="I43" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44">
+        <v>100</v>
+      </c>
+      <c r="I44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45">
+        <v>40</v>
+      </c>
+      <c r="I45" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add reddick appendix.  test embedded model
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02946E4-3609-4F0B-A805-9EE244014FCF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2DE576-8090-4C84-8FD6-9D7A67847525}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="76">
   <si>
     <t>hab_value</t>
   </si>
@@ -614,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1199,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1361,8 +1361,11 @@
       <c r="G40" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1381,11 +1384,17 @@
       <c r="G41" t="s">
         <v>51</v>
       </c>
+      <c r="H41" t="s">
+        <v>70</v>
+      </c>
       <c r="I41" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>58</v>
       </c>
@@ -1402,7 +1411,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>59</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>60</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
clean up and post running fragment
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5662967F-B9EC-4BB6-8445-FB8245A9D004}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37689432-F551-4D7E-9FB3-11EF2B44CDA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
   <si>
     <t>hab_value</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>RB, CT</t>
+  </si>
+  <si>
+    <t>RB, CT, CO, BT</t>
+  </si>
+  <si>
+    <t>RB, CO</t>
   </si>
 </sst>
 </file>
@@ -621,7 +627,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1281,8 +1287,17 @@
       <c r="E36" t="s">
         <v>51</v>
       </c>
+      <c r="H36" t="s">
+        <v>69</v>
+      </c>
       <c r="I36" t="s">
         <v>70</v>
+      </c>
+      <c r="K36">
+        <v>780</v>
+      </c>
+      <c r="L36" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -1330,8 +1345,11 @@
       <c r="I38" t="s">
         <v>70</v>
       </c>
+      <c r="K38">
+        <v>1000</v>
+      </c>
       <c r="L38" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
@@ -1417,10 +1435,22 @@
         <v>72</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>180</v>
+      </c>
+      <c r="G42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H42" t="s">
+        <v>69</v>
       </c>
       <c r="I42" t="s">
         <v>70</v>
+      </c>
+      <c r="K42">
+        <v>4500</v>
+      </c>
+      <c r="L42" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add a rough richfield
</commit_message>
<xml_diff>
--- a/data/habitat_confirmations_priorities.xlsx
+++ b/data/habitat_confirmations_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\fish_passage_bulkley_2020_reporting\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37689432-F551-4D7E-9FB3-11EF2B44CDA5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD973B2E-6178-4045-8F8B-D83F1A8A02B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="81">
   <si>
     <t>hab_value</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>RB, CO</t>
+  </si>
+  <si>
+    <t>CH,CO,LNC,LSU,RB,ST</t>
   </si>
 </sst>
 </file>
@@ -626,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -884,8 +887,17 @@
       <c r="F13" t="s">
         <v>51</v>
       </c>
+      <c r="H13" t="s">
+        <v>70</v>
+      </c>
       <c r="I13" t="s">
         <v>70</v>
+      </c>
+      <c r="K13">
+        <v>2000</v>
+      </c>
+      <c r="L13" t="s">
+        <v>80</v>
       </c>
       <c r="M13" t="s">
         <v>51</v>
@@ -907,6 +919,9 @@
       <c r="F14" t="s">
         <v>51</v>
       </c>
+      <c r="H14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1270,6 +1285,9 @@
       <c r="E35" t="s">
         <v>51</v>
       </c>
+      <c r="H35" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -1319,6 +1337,9 @@
       <c r="F37" t="s">
         <v>51</v>
       </c>
+      <c r="H37" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
@@ -1342,6 +1363,9 @@
       <c r="G38" t="s">
         <v>51</v>
       </c>
+      <c r="H38" t="s">
+        <v>69</v>
+      </c>
       <c r="I38" t="s">
         <v>70</v>
       </c>
@@ -1367,6 +1391,9 @@
       </c>
       <c r="G39" t="s">
         <v>51</v>
+      </c>
+      <c r="H39" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>